<commit_message>
Auto update on 2025-12-22 18:56:30
</commit_message>
<xml_diff>
--- a/jama_exports/kp_data.xlsx
+++ b/jama_exports/kp_data.xlsx
@@ -1142,10 +1142,10 @@
         <v>7</v>
       </c>
       <c r="P12">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Q12">
-        <v>3.17</v>
+        <v>3.2</v>
       </c>
       <c r="R12">
         <v>0.02</v>

</xml_diff>

<commit_message>
Auto update on 2025-12-23 10:17:36
</commit_message>
<xml_diff>
--- a/jama_exports/kp_data.xlsx
+++ b/jama_exports/kp_data.xlsx
@@ -664,7 +664,7 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G4">
         <v>4</v>
@@ -688,7 +688,7 @@
         <v>7</v>
       </c>
       <c r="N4">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="O4">
         <v>11</v>
@@ -697,7 +697,7 @@
         <v>114</v>
       </c>
       <c r="Q4">
-        <v>2.98</v>
+        <v>2.99</v>
       </c>
       <c r="R4">
         <v>0.03</v>
@@ -788,7 +788,7 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="K6">
         <v>60</v>
@@ -800,7 +800,7 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="O6">
         <v>60</v>
@@ -809,7 +809,7 @@
         <v>82</v>
       </c>
       <c r="Q6">
-        <v>4.76</v>
+        <v>4.78</v>
       </c>
       <c r="R6">
         <v>0.15</v>

</xml_diff>

<commit_message>
Auto update on 2025-12-23 14:45:07
</commit_message>
<xml_diff>
--- a/jama_exports/kp_data.xlsx
+++ b/jama_exports/kp_data.xlsx
@@ -611,7 +611,7 @@
         <v>230</v>
       </c>
       <c r="G3">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -635,7 +635,7 @@
         <v>230</v>
       </c>
       <c r="O3">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="P3">
         <v>96</v>
@@ -644,7 +644,7 @@
         <v>2.4</v>
       </c>
       <c r="R3">
-        <v>0.38</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -664,7 +664,7 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G4">
         <v>4</v>
@@ -688,7 +688,7 @@
         <v>7</v>
       </c>
       <c r="N4">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="O4">
         <v>11</v>
@@ -697,7 +697,7 @@
         <v>114</v>
       </c>
       <c r="Q4">
-        <v>2.99</v>
+        <v>2.97</v>
       </c>
       <c r="R4">
         <v>0.03</v>
@@ -720,7 +720,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G5">
         <v>13</v>
@@ -744,7 +744,7 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="O5">
         <v>13</v>
@@ -753,7 +753,7 @@
         <v>64</v>
       </c>
       <c r="Q5">
-        <v>2.31</v>
+        <v>2.33</v>
       </c>
       <c r="R5">
         <v>0.09</v>
@@ -788,7 +788,7 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="K6">
         <v>60</v>
@@ -800,16 +800,16 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="O6">
         <v>60</v>
       </c>
       <c r="P6">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="Q6">
-        <v>4.78</v>
+        <v>4.77</v>
       </c>
       <c r="R6">
         <v>0.15</v>
@@ -844,7 +844,7 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="K7">
         <v>41</v>
@@ -856,7 +856,7 @@
         <v>0</v>
       </c>
       <c r="N7">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="O7">
         <v>43</v>
@@ -865,7 +865,7 @@
         <v>95</v>
       </c>
       <c r="Q7">
-        <v>4.27</v>
+        <v>4.26</v>
       </c>
       <c r="R7">
         <v>0.11</v>
@@ -1003,7 +1003,7 @@
         <v>242</v>
       </c>
       <c r="G10">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -1027,7 +1027,7 @@
         <v>242</v>
       </c>
       <c r="O10">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="P10">
         <v>76</v>
@@ -1036,7 +1036,7 @@
         <v>3.18</v>
       </c>
       <c r="R10">
-        <v>0.35</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="11" spans="1:18">
@@ -1168,7 +1168,7 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G13">
         <v>14</v>
@@ -1192,16 +1192,16 @@
         <v>0</v>
       </c>
       <c r="N13">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="O13">
         <v>14</v>
       </c>
       <c r="P13">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="Q13">
-        <v>2.62</v>
+        <v>2.61</v>
       </c>
       <c r="R13">
         <v>0.12</v>
@@ -1280,7 +1280,7 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G15">
         <v>8</v>
@@ -1304,7 +1304,7 @@
         <v>0</v>
       </c>
       <c r="N15">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O15">
         <v>8</v>
@@ -1313,7 +1313,7 @@
         <v>27</v>
       </c>
       <c r="Q15">
-        <v>3.07</v>
+        <v>3.04</v>
       </c>
       <c r="R15">
         <v>0.1</v>
@@ -1392,7 +1392,7 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -1416,16 +1416,16 @@
         <v>0</v>
       </c>
       <c r="N17">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="O17">
         <v>0</v>
       </c>
       <c r="P17">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q17">
-        <v>3.17</v>
+        <v>3.57</v>
       </c>
       <c r="R17">
         <v>0</v>

</xml_diff>

<commit_message>
Auto update on 2025-12-24 15:08:26
</commit_message>
<xml_diff>
--- a/jama_exports/kp_data.xlsx
+++ b/jama_exports/kp_data.xlsx
@@ -611,7 +611,7 @@
         <v>230</v>
       </c>
       <c r="G3">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -635,7 +635,7 @@
         <v>230</v>
       </c>
       <c r="O3">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="P3">
         <v>96</v>
@@ -644,7 +644,7 @@
         <v>2.4</v>
       </c>
       <c r="R3">
-        <v>0.39</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -694,10 +694,10 @@
         <v>11</v>
       </c>
       <c r="P4">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="Q4">
-        <v>2.97</v>
+        <v>2.95</v>
       </c>
       <c r="R4">
         <v>0.03</v>
@@ -788,7 +788,7 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>396</v>
+        <v>414</v>
       </c>
       <c r="K6">
         <v>60</v>
@@ -800,7 +800,7 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>396</v>
+        <v>414</v>
       </c>
       <c r="O6">
         <v>60</v>
@@ -809,10 +809,10 @@
         <v>83</v>
       </c>
       <c r="Q6">
-        <v>4.77</v>
+        <v>4.99</v>
       </c>
       <c r="R6">
-        <v>0.15</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="7" spans="1:18">
@@ -862,10 +862,10 @@
         <v>43</v>
       </c>
       <c r="P7">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q7">
-        <v>4.26</v>
+        <v>4.22</v>
       </c>
       <c r="R7">
         <v>0.11</v>
@@ -944,7 +944,7 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="G9">
         <v>20</v>
@@ -968,16 +968,16 @@
         <v>0</v>
       </c>
       <c r="N9">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="O9">
         <v>20</v>
       </c>
       <c r="P9">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="Q9">
-        <v>2.49</v>
+        <v>2.47</v>
       </c>
       <c r="R9">
         <v>0.1</v>
@@ -1000,10 +1000,10 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="G10">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -1024,13 +1024,13 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="O10">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="P10">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="Q10">
         <v>3.18</v>
@@ -1056,7 +1056,7 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G11">
         <v>3</v>
@@ -1080,16 +1080,16 @@
         <v>0</v>
       </c>
       <c r="N11">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="O11">
         <v>3</v>
       </c>
       <c r="P11">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q11">
-        <v>2.04</v>
+        <v>2</v>
       </c>
       <c r="R11">
         <v>0.06</v>
@@ -1112,7 +1112,7 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G12">
         <v>7</v>
@@ -1136,16 +1136,16 @@
         <v>0</v>
       </c>
       <c r="N12">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="O12">
         <v>7</v>
       </c>
       <c r="P12">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="Q12">
-        <v>3.2</v>
+        <v>3.18</v>
       </c>
       <c r="R12">
         <v>0.02</v>
@@ -1224,7 +1224,7 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="G14">
         <v>52</v>
@@ -1248,16 +1248,16 @@
         <v>0</v>
       </c>
       <c r="N14">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="O14">
         <v>52</v>
       </c>
       <c r="P14">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q14">
-        <v>3.35</v>
+        <v>3.33</v>
       </c>
       <c r="R14">
         <v>0.16</v>
@@ -1280,7 +1280,7 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G15">
         <v>8</v>
@@ -1304,19 +1304,19 @@
         <v>0</v>
       </c>
       <c r="N15">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="O15">
         <v>8</v>
       </c>
       <c r="P15">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q15">
         <v>3.04</v>
       </c>
       <c r="R15">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="16" spans="1:18">
@@ -1336,7 +1336,7 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G16">
         <v>7</v>
@@ -1360,19 +1360,19 @@
         <v>0</v>
       </c>
       <c r="N16">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O16">
         <v>7</v>
       </c>
       <c r="P16">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q16">
-        <v>1.7</v>
+        <v>1.68</v>
       </c>
       <c r="R16">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="17" spans="1:18">
@@ -1392,7 +1392,7 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -1416,16 +1416,16 @@
         <v>0</v>
       </c>
       <c r="N17">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="O17">
         <v>0</v>
       </c>
       <c r="P17">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q17">
-        <v>3.57</v>
+        <v>3.5</v>
       </c>
       <c r="R17">
         <v>0</v>

</xml_diff>

<commit_message>
Auto update on 2026-01-08 11:56:14
</commit_message>
<xml_diff>
--- a/jama_exports/kp_data.xlsx
+++ b/jama_exports/kp_data.xlsx
@@ -611,7 +611,7 @@
         <v>230</v>
       </c>
       <c r="G3">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -635,7 +635,7 @@
         <v>230</v>
       </c>
       <c r="O3">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="P3">
         <v>96</v>
@@ -644,7 +644,7 @@
         <v>2.4</v>
       </c>
       <c r="R3">
-        <v>0.4</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -664,7 +664,7 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G4">
         <v>4</v>
@@ -688,16 +688,16 @@
         <v>7</v>
       </c>
       <c r="N4">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="O4">
         <v>11</v>
       </c>
       <c r="P4">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Q4">
-        <v>2.95</v>
+        <v>2.96</v>
       </c>
       <c r="R4">
         <v>0.03</v>
@@ -788,7 +788,7 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>414</v>
+        <v>438</v>
       </c>
       <c r="K6">
         <v>60</v>
@@ -800,16 +800,16 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>414</v>
+        <v>438</v>
       </c>
       <c r="O6">
         <v>60</v>
       </c>
       <c r="P6">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="Q6">
-        <v>4.99</v>
+        <v>5.09</v>
       </c>
       <c r="R6">
         <v>0.14</v>
@@ -826,7 +826,7 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -844,7 +844,7 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K7">
         <v>41</v>
@@ -856,19 +856,19 @@
         <v>0</v>
       </c>
       <c r="N7">
-        <v>405</v>
+        <v>416</v>
       </c>
       <c r="O7">
         <v>43</v>
       </c>
       <c r="P7">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="Q7">
-        <v>4.22</v>
+        <v>4.24</v>
       </c>
       <c r="R7">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="8" spans="1:18">
@@ -944,7 +944,7 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G9">
         <v>20</v>
@@ -968,7 +968,7 @@
         <v>0</v>
       </c>
       <c r="N9">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="O9">
         <v>20</v>
@@ -977,7 +977,7 @@
         <v>79</v>
       </c>
       <c r="Q9">
-        <v>2.47</v>
+        <v>2.44</v>
       </c>
       <c r="R9">
         <v>0.1</v>
@@ -1000,10 +1000,10 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="G10">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -1024,16 +1024,16 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="O10">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="P10">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="Q10">
-        <v>3.18</v>
+        <v>3.17</v>
       </c>
       <c r="R10">
         <v>0.36</v>
@@ -1056,7 +1056,7 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G11">
         <v>3</v>
@@ -1080,16 +1080,16 @@
         <v>0</v>
       </c>
       <c r="N11">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O11">
         <v>3</v>
       </c>
       <c r="P11">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q11">
-        <v>2</v>
+        <v>2.04</v>
       </c>
       <c r="R11">
         <v>0.06</v>
@@ -1112,7 +1112,7 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="G12">
         <v>7</v>
@@ -1136,13 +1136,13 @@
         <v>0</v>
       </c>
       <c r="N12">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="O12">
         <v>7</v>
       </c>
       <c r="P12">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="Q12">
         <v>3.18</v>
@@ -1168,7 +1168,7 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="G13">
         <v>14</v>
@@ -1192,19 +1192,19 @@
         <v>0</v>
       </c>
       <c r="N13">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="O13">
         <v>14</v>
       </c>
       <c r="P13">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="Q13">
-        <v>2.61</v>
+        <v>2.67</v>
       </c>
       <c r="R13">
-        <v>0.12</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="14" spans="1:18">
@@ -1224,10 +1224,10 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <v>320</v>
+        <v>331</v>
       </c>
       <c r="G14">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -1248,19 +1248,19 @@
         <v>0</v>
       </c>
       <c r="N14">
-        <v>320</v>
+        <v>331</v>
       </c>
       <c r="O14">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="P14">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="Q14">
-        <v>3.33</v>
+        <v>3.31</v>
       </c>
       <c r="R14">
-        <v>0.16</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="15" spans="1:18">
@@ -1280,10 +1280,10 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G15">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H15">
         <v>43</v>
@@ -1304,16 +1304,16 @@
         <v>0</v>
       </c>
       <c r="N15">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="O15">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="P15">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="Q15">
-        <v>3.04</v>
+        <v>2.97</v>
       </c>
       <c r="R15">
         <v>0.09</v>
@@ -1336,10 +1336,10 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G16">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H16">
         <v>3</v>
@@ -1360,19 +1360,19 @@
         <v>0</v>
       </c>
       <c r="N16">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="O16">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="P16">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Q16">
-        <v>1.68</v>
+        <v>1.67</v>
       </c>
       <c r="R16">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="17" spans="1:18">
@@ -1392,7 +1392,7 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -1416,7 +1416,7 @@
         <v>0</v>
       </c>
       <c r="N17">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O17">
         <v>0</v>
@@ -1425,7 +1425,7 @@
         <v>8</v>
       </c>
       <c r="Q17">
-        <v>3.5</v>
+        <v>3.62</v>
       </c>
       <c r="R17">
         <v>0</v>

</xml_diff>

<commit_message>
Auto update on 2026-02-25 15:43:53
</commit_message>
<xml_diff>
--- a/jama_exports/kp_data.xlsx
+++ b/jama_exports/kp_data.xlsx
@@ -70,6 +70,9 @@
     <t>Dinesh</t>
   </si>
   <si>
+    <t>Harini Sri</t>
+  </si>
+  <si>
     <t>Veeramanikandan</t>
   </si>
   <si>
@@ -83,9 +86,6 @@
   </si>
   <si>
     <t>Priyavalli</t>
-  </si>
-  <si>
-    <t>Harini Sri</t>
   </si>
   <si>
     <t>Suryanarayanan</t>
@@ -528,25 +528,25 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="I2">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="J2">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="K2">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="L2">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="M2">
-        <v>4.56</v>
+        <v>4.24</v>
       </c>
       <c r="N2">
-        <v>0.26</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -566,10 +566,10 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H3">
         <v>79</v>
@@ -578,19 +578,19 @@
         <v>5</v>
       </c>
       <c r="J3">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="K3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L3">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="M3">
-        <v>5.29</v>
+        <v>4.9</v>
       </c>
       <c r="N3">
-        <v>0.06</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -616,25 +616,25 @@
         <v>1</v>
       </c>
       <c r="H4">
+        <v>19</v>
+      </c>
+      <c r="I4">
+        <v>8</v>
+      </c>
+      <c r="J4">
+        <v>24</v>
+      </c>
+      <c r="K4">
         <v>9</v>
       </c>
-      <c r="I4">
-        <v>6</v>
-      </c>
-      <c r="J4">
+      <c r="L4">
         <v>14</v>
       </c>
-      <c r="K4">
-        <v>7</v>
-      </c>
-      <c r="L4">
-        <v>10</v>
-      </c>
       <c r="M4">
-        <v>1.4</v>
+        <v>1.71</v>
       </c>
       <c r="N4">
-        <v>0.5</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -654,10 +654,10 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="G5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -666,16 +666,16 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="K5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L5">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="M5">
-        <v>3.47</v>
+        <v>3.48</v>
       </c>
       <c r="N5">
         <v>0.08</v>
@@ -698,10 +698,10 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -710,19 +710,19 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K6">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="L6">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="M6">
-        <v>2.09</v>
+        <v>1.6</v>
       </c>
       <c r="N6">
-        <v>0.09</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -736,16 +736,16 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="G7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -754,19 +754,19 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="K7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L7">
         <v>11</v>
       </c>
       <c r="M7">
-        <v>1.55</v>
+        <v>2.09</v>
       </c>
       <c r="N7">
-        <v>0.18</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -780,16 +780,16 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="G8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -798,19 +798,19 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="K8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L8">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M8">
-        <v>1.86</v>
+        <v>2</v>
       </c>
       <c r="N8">
-        <v>0.15</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -830,10 +830,10 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>85</v>
+        <v>32</v>
       </c>
       <c r="G9">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -842,19 +842,19 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>85</v>
+        <v>32</v>
       </c>
       <c r="K9">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="L9">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M9">
-        <v>4.47</v>
+        <v>1.88</v>
       </c>
       <c r="N9">
-        <v>0.18</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -874,10 +874,10 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>28</v>
+        <v>98</v>
       </c>
       <c r="G10">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -886,19 +886,19 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>28</v>
+        <v>98</v>
       </c>
       <c r="K10">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="L10">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="M10">
-        <v>2.33</v>
+        <v>4.45</v>
       </c>
       <c r="N10">
-        <v>0.39</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -918,10 +918,10 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="G11">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -930,19 +930,19 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="K11">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L11">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="M11">
-        <v>1.1</v>
+        <v>2.33</v>
       </c>
       <c r="N11">
-        <v>1.27</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -962,10 +962,10 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="G12">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -974,19 +974,19 @@
         <v>0</v>
       </c>
       <c r="J12">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="K12">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="L12">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="M12">
-        <v>1.73</v>
+        <v>2.29</v>
       </c>
       <c r="N12">
-        <v>2.32</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -1006,7 +1006,7 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="G13">
         <v>3</v>
@@ -1018,19 +1018,19 @@
         <v>0</v>
       </c>
       <c r="J13">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="K13">
         <v>3</v>
       </c>
       <c r="L13">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="M13">
-        <v>1.62</v>
+        <v>1.75</v>
       </c>
       <c r="N13">
-        <v>0.23</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -1050,7 +1050,7 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -1062,16 +1062,16 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="K14">
         <v>0</v>
       </c>
       <c r="L14">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="M14">
-        <v>2.9</v>
+        <v>2.75</v>
       </c>
       <c r="N14">
         <v>0</v>
@@ -1094,10 +1094,10 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -1106,19 +1106,19 @@
         <v>0</v>
       </c>
       <c r="J15">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L15">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M15">
-        <v>3.12</v>
+        <v>3.4</v>
       </c>
       <c r="N15">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
   </sheetData>

</xml_diff>